<commit_message>
RAF data update to support forthcoming changes to capacity credit values.
</commit_message>
<xml_diff>
--- a/InputData/elec/RAF/Regional Availability Factor.xlsx
+++ b/InputData/elec/RAF/Regional Availability Factor.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\RAF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\RAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AC669C-A089-43AC-8C3F-D19C2C3202FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38BA603-0BA4-4B13-8D82-C234526C7A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
+    <workbookView xWindow="29895" yWindow="4140" windowWidth="26325" windowHeight="17235" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RAF-generation" sheetId="2" r:id="rId2"/>
     <sheet name="RAF-demand-altering-techs" sheetId="3" r:id="rId3"/>
+    <sheet name="RAF-capacity" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <t>Source:</t>
   </si>
@@ -127,9 +128,6 @@
     <t>known as a theoretical "copper sheet."  In reality, transmission and distribution</t>
   </si>
   <si>
-    <t>constrain electricity flows.</t>
-  </si>
-  <si>
     <t>The EPS groups power plants by type (for instance, all natural gas combined cycle</t>
   </si>
   <si>
@@ -154,12 +152,6 @@
     <t>not already incorporated into the capacity factors of the plants themselves.</t>
   </si>
   <si>
-    <t>This variable allows you to specify a regional availability factor (RAF).  When</t>
-  </si>
-  <si>
-    <t>the RAF is less than 1, it reduces the amount of capacity available that can</t>
-  </si>
-  <si>
     <t>meet demand due to regional factors such as transmission constraints, i.e.,</t>
   </si>
   <si>
@@ -194,6 +186,48 @@
   </si>
   <si>
     <t>hydrogen combined cycle</t>
+  </si>
+  <si>
+    <t>Unit: dimensionless (% of capacity credit allowed)</t>
+  </si>
+  <si>
+    <t>capacity credit multiplier</t>
+  </si>
+  <si>
+    <t>RAF Regional Availability Factor for Capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constrain electricity flows. Furthemore, there are important regional differences </t>
+  </si>
+  <si>
+    <t>in capacity factor and land availability for variable renewable electricity technologies.</t>
+  </si>
+  <si>
+    <t>These must be accounted for when estimating what types of new resources are built</t>
+  </si>
+  <si>
+    <t>This variable allows you to specify a regional availability factor (RAF) for generation and</t>
+  </si>
+  <si>
+    <t>capacity.  When the RAF is less than 1, it reduces the amount of capacity available that can</t>
+  </si>
+  <si>
+    <t>The RAF for capacity reduces the value of the capacity credit a resource receives</t>
+  </si>
+  <si>
+    <t>in the reliability capacity addition mechanism. This is to account for the differeing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity factors of variable renewable technologies by region and their limited </t>
+  </si>
+  <si>
+    <t xml:space="preserve">geographcial availability, often near load centers. It can be used as a </t>
+  </si>
+  <si>
+    <t>stand-in for the fact that the model does not currently have subregional detail</t>
+  </si>
+  <si>
+    <t>for the electricity sector.</t>
   </si>
 </sst>
 </file>
@@ -565,133 +599,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667665C7-8A8E-46D9-B686-64BA7741F669}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -703,12 +784,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D9ED82-0D6D-4554-A249-670AA724E405}">
   <sheetPr>
-    <tabColor theme="4" tint="-0.249977111117893"/>
+    <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A25"/>
+      <selection sqref="A1:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +983,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B24">
         <v>0.9</v>
@@ -910,7 +991,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B25">
         <v>0.9</v>
@@ -924,11 +1005,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46AF6E62-1D44-4071-9B4B-8D8AD9AB16B0}">
   <sheetPr>
-    <tabColor theme="4" tint="-0.249977111117893"/>
+    <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -946,10 +1029,231 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED7E3B8-DB01-4BFB-908D-32A466D537CF}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>47</v>
       </c>
-      <c r="B2">
-        <v>0.9</v>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Input data updates to correclty factor in capacity factor improvements for new capacity and adjust the RAF for capacity
</commit_message>
<xml_diff>
--- a/InputData/elec/RAF/Regional Availability Factor.xlsx
+++ b/InputData/elec/RAF/Regional Availability Factor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\RAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38BA603-0BA4-4B13-8D82-C234526C7A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EEE36A-44E1-43F8-B3DC-C40773C3587B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29895" yWindow="4140" windowWidth="26325" windowHeight="17235" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
+    <workbookView xWindow="30585" yWindow="4830" windowWidth="26325" windowHeight="17235" activeTab="3" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -601,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667665C7-8A8E-46D9-B686-64BA7741F669}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
@@ -1047,17 +1047,14 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>49</v>
       </c>
       <c r="B1" t="s">
@@ -1101,7 +1098,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1109,7 +1106,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1117,7 +1114,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1125,7 +1122,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1133,7 +1130,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1173,7 +1170,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Calibration edits for elec/RAF
</commit_message>
<xml_diff>
--- a/InputData/elec/RAF/Regional Availability Factor.xlsx
+++ b/InputData/elec/RAF/Regional Availability Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\RAF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\RAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EEE36A-44E1-43F8-B3DC-C40773C3587B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF44064-37B5-4C2B-AEB8-24E36A7FA459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30585" yWindow="4830" windowWidth="26325" windowHeight="17235" activeTab="3" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667665C7-8A8E-46D9-B686-64BA7741F669}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +789,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B25"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +874,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -882,7 +882,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1047,7 +1047,7 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update RAF values for hydrogen plants as they would need access to hydrogen pipeline supplier, which doesn't currently exist.
</commit_message>
<xml_diff>
--- a/InputData/elec/RAF/Regional Availability Factor.xlsx
+++ b/InputData/elec/RAF/Regional Availability Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\RAF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\RAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF44064-37B5-4C2B-AEB8-24E36A7FA459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71882C16-618B-4A9B-B33D-02C579EB9193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
+    <workbookView xWindow="1545" yWindow="1335" windowWidth="20985" windowHeight="14580" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
   <si>
     <t>Source:</t>
   </si>
@@ -228,6 +228,18 @@
   </si>
   <si>
     <t>for the electricity sector.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We also apply a very low credit for hydrogen plants because they require </t>
+  </si>
+  <si>
+    <t xml:space="preserve">access to a hydrogen supplier, most likely pipeline deliery, which </t>
+  </si>
+  <si>
+    <t xml:space="preserve">does not exist in the US today and they would only be used in certain </t>
+  </si>
+  <si>
+    <t>unique circumstances.</t>
   </si>
 </sst>
 </file>
@@ -303,9 +315,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -343,7 +355,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -449,7 +461,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -591,7 +603,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -599,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667665C7-8A8E-46D9-B686-64BA7741F669}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:A48"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,6 +785,26 @@
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1048,7 +1080,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,7 +1274,7 @@
         <v>47</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1250,7 +1282,7 @@
         <v>48</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to code for capacity factors and clean firm.
</commit_message>
<xml_diff>
--- a/InputData/elec/RAF/Regional Availability Factor.xlsx
+++ b/InputData/elec/RAF/Regional Availability Factor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\RAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71882C16-618B-4A9B-B33D-02C579EB9193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D10B98B-3B2C-474A-898A-D6B427FCD2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="1335" windowWidth="20985" windowHeight="14580" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="3" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -613,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667665C7-8A8E-46D9-B686-64BA7741F669}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -1079,8 +1079,8 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,7 +1274,7 @@
         <v>47</v>
       </c>
       <c r="B24">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
         <v>48</v>
       </c>
       <c r="B25">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update coal RAF, bgdpbes
</commit_message>
<xml_diff>
--- a/InputData/elec/RAF/Regional Availability Factor.xlsx
+++ b/InputData/elec/RAF/Regional Availability Factor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\elec\RAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C12635-1DB5-4D74-846D-2C39CF96E070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A59768-112B-4192-A607-1839462A1F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="570" windowWidth="12330" windowHeight="16680" activeTab="1" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="20025" windowHeight="16860" activeTab="1" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -821,7 +821,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Moves fuel prices to be mapped by Future Year and adds five year future price average for electricity sector calculations. This lets us proejct average 5 year revenue for plant types instead of relying on historical data. This is a big improvement that helps with new capacity additions.
</commit_message>
<xml_diff>
--- a/InputData/elec/RAF/Regional Availability Factor.xlsx
+++ b/InputData/elec/RAF/Regional Availability Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\elec\RAF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\RAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A59768-112B-4192-A607-1839462A1F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CC6B04-B346-4890-A318-734C137A4431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="20025" windowHeight="16860" activeTab="1" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="1" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -821,7 +821,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,8 +829,8 @@
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
@@ -842,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.6</v>
+        <v>0.46666666699999998</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -850,7 +850,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -858,7 +858,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,7 +922,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -930,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -946,7 +946,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -962,7 +962,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -970,7 +970,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Increase RAF for peaker plants from 0.7 to 1
</commit_message>
<xml_diff>
--- a/InputData/elec/RAF/Regional Availability Factor.xlsx
+++ b/InputData/elec/RAF/Regional Availability Factor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\RAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CC6B04-B346-4890-A318-734C137A4431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E197654D-E8CD-48D0-94A6-D59B31D7746C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="1" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -613,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667665C7-8A8E-46D9-B686-64BA7741F669}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -820,8 +820,8 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +922,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -930,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated RAF values for generation
</commit_message>
<xml_diff>
--- a/InputData/elec/RAF/Regional Availability Factor.xlsx
+++ b/InputData/elec/RAF/Regional Availability Factor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\RAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E197654D-E8CD-48D0-94A6-D59B31D7746C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B03590-6867-428B-B57F-2015C6EA0F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
+    <workbookView xWindow="2310" yWindow="195" windowWidth="22875" windowHeight="23115" activeTab="1" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -613,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667665C7-8A8E-46D9-B686-64BA7741F669}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -820,8 +820,8 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.46666666699999998</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -850,7 +850,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.7</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -858,7 +858,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.7</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>